<commit_message>
Final update for assignment 2
</commit_message>
<xml_diff>
--- a/Assignment2/Results/table_2.xlsx
+++ b/Assignment2/Results/table_2.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine CHEHIRE\Documents\GitHub\Deep_1_AC_AN_PW\Assignment2\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B229E714-856A-4D92-A393-2F5ACE1E5516}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>train ppl</t>
   </si>
@@ -29,6 +35,15 @@
   </si>
   <si>
     <t>g3_gru_sgd</t>
+  </si>
+  <si>
+    <t>g4_gru_sgd_hyp1</t>
+  </si>
+  <si>
+    <t>g5_gru_sgd_hyp2</t>
+  </si>
+  <si>
+    <t>g6_gru_sgd_hyp3</t>
   </si>
   <si>
     <t>r1_rnn_adam</t>
@@ -70,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,7 +111,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -111,11 +126,172 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -123,17 +299,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -180,7 +422,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,9 +454,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,6 +506,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,187 +699,246 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="G5:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
+    <row r="5" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="7" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>59.64785271323299</v>
-      </c>
-      <c r="C2">
-        <v>111.1894507099477</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="H7" s="1">
+        <v>59.647852713232993</v>
+      </c>
+      <c r="I7" s="8">
+        <v>111.18945070994771</v>
+      </c>
+    </row>
+    <row r="8" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>65.52901838369723</v>
-      </c>
-      <c r="C3">
+      <c r="H8" s="2">
+        <v>65.529018383697235</v>
+      </c>
+      <c r="I8" s="9">
         <v>103.0605655628399</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="9" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>50.12297898151582</v>
-      </c>
-      <c r="C4">
-        <v>113.3937101338605</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="H9" s="2">
+        <v>50.122978981515821</v>
+      </c>
+      <c r="I9" s="9">
+        <v>113.39371013386049</v>
+      </c>
+    </row>
+    <row r="10" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>120.6246336655607</v>
-      </c>
-      <c r="C5">
-        <v>156.3533450812893</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="H10" s="2">
+        <v>67.033475019813466</v>
+      </c>
+      <c r="I10" s="9">
+        <v>110.7441025542503</v>
+      </c>
+    </row>
+    <row r="11" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="H11" s="2">
+        <v>70.248376652642762</v>
+      </c>
+      <c r="I11" s="9">
+        <v>113.61605546811521</v>
+      </c>
+    </row>
+    <row r="12" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="3">
+        <v>45.869858367398457</v>
+      </c>
+      <c r="I12" s="10">
+        <v>108.58378422593501</v>
+      </c>
+    </row>
+    <row r="13" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1">
+        <v>120.62463366556069</v>
+      </c>
+      <c r="I13" s="8">
+        <v>156.35334508128929</v>
+      </c>
+    </row>
+    <row r="14" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="2">
         <v>229.7823922746897</v>
       </c>
-      <c r="C6">
-        <v>195.8752376229444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>2965.429085747329</v>
-      </c>
-      <c r="C7">
-        <v>2188.200816209259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+      <c r="I14" s="9">
+        <v>195.87523762294441</v>
+      </c>
+    </row>
+    <row r="15" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2965.4290857473288</v>
+      </c>
+      <c r="I15" s="9">
+        <v>2188.2008162092588</v>
+      </c>
+    </row>
+    <row r="16" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="2">
         <v>145.4764217556702</v>
       </c>
-      <c r="C8">
-        <v>152.2164744509163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>190.6901878180983</v>
-      </c>
-      <c r="C9">
+      <c r="I16" s="9">
+        <v>152.21647445091631</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="2">
+        <v>190.69018781809831</v>
+      </c>
+      <c r="I17" s="9">
         <v>195.8634087609822</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3">
         <v>131.5435345585523</v>
       </c>
-      <c r="C10">
+      <c r="I18" s="10">
         <v>149.369937630675</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>3.415880712567909</v>
-      </c>
-      <c r="C11">
-        <v>138.1508929122591</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>60.41347239443049</v>
-      </c>
-      <c r="C12">
-        <v>143.8101244159508</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>29.29684124736197</v>
-      </c>
-      <c r="C13">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.4158807125679091</v>
+      </c>
+      <c r="I19" s="8">
+        <v>138.15089291225911</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2">
+        <v>60.413472394430492</v>
+      </c>
+      <c r="I20" s="9">
+        <v>143.81012441595081</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2">
+        <v>29.296841247361971</v>
+      </c>
+      <c r="I21" s="9">
         <v>171.4813792984678</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>83.80661048799902</v>
-      </c>
-      <c r="C14">
+    <row r="22" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="2">
+        <v>83.806610487999023</v>
+      </c>
+      <c r="I22" s="9">
         <v>147.6290604537439</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
+    <row r="23" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="2">
         <v>15.44566639505314</v>
       </c>
-      <c r="C15">
-        <v>159.0059594884285</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>74.65831688304941</v>
-      </c>
-      <c r="C16">
-        <v>152.3507673756783</v>
+      <c r="I23" s="9">
+        <v>159.00595948842849</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13">
+        <v>74.658316883049409</v>
+      </c>
+      <c r="I24" s="14">
+        <v>152.35076737567829</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H7:H12">
+    <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:I12">
+    <cfRule type="top10" dxfId="4" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13:H18">
+    <cfRule type="top10" dxfId="3" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I18">
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19:H24">
+    <cfRule type="top10" dxfId="1" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I19:I24">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>